<commit_message>
Added the ability to convert the first word of a sentence to lowercase
</commit_message>
<xml_diff>
--- a/databank_englishB.xlsx
+++ b/databank_englishB.xlsx
@@ -237,7 +237,7 @@
     <t>瀕死の鯨は奇跡的に回復しました。</t>
   </si>
   <si>
-    <t>The dying whale whale miraculously recovered.</t>
+    <t>The dying whale miraculously recovered.</t>
   </si>
   <si>
     <t>私はあなたのものに似たようなドレスを探している。</t>
@@ -420,7 +420,7 @@
     <t>All the students sat down and began to talk to each other.</t>
   </si>
   <si>
-    <t>私はどこにいくかものにをするかも分からなかった。</t>
+    <t>私は何処にいくかも何をするかも分からなかった。</t>
   </si>
   <si>
     <t>I didn’t know where to go or what to do.</t>
@@ -699,7 +699,7 @@
     <t>母の腕時計はスイス製だ。</t>
   </si>
   <si>
-    <t>My mother’s watch in made in Switzerland.</t>
+    <t>My mother’s watch is made in Switzerland.</t>
   </si>
   <si>
     <t>あのカバンは何でできているのですか。</t>
@@ -1023,7 +1023,7 @@
     <t>私の母は私にどこにいたのか尋ねた。</t>
   </si>
   <si>
-    <t>My mother asked asked me where I had been?</t>
+    <t>My mother asked me where I had been?</t>
   </si>
   <si>
     <t>その配達員の男性は次の日に戻ってくると言った。</t>
@@ -1087,7 +1087,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1097,7 +1097,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -1113,14 +1112,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2586,7 +2582,7 @@
       <c r="C89" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89" s="1">
         <v>89.0</v>
       </c>
     </row>
@@ -2600,7 +2596,7 @@
       <c r="C90" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90" s="1">
         <v>90.0</v>
       </c>
     </row>
@@ -2611,10 +2607,10 @@
       <c r="B91" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91" s="1">
         <v>91.0</v>
       </c>
     </row>
@@ -2628,7 +2624,7 @@
       <c r="C92" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92" s="1">
         <v>92.0</v>
       </c>
     </row>
@@ -2642,7 +2638,7 @@
       <c r="C93" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93" s="1">
         <v>93.0</v>
       </c>
     </row>
@@ -2653,10 +2649,10 @@
       <c r="B94" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E94" s="1">
         <v>94.0</v>
       </c>
     </row>
@@ -2670,7 +2666,7 @@
       <c r="C95" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E95" s="1">
         <v>95.0</v>
       </c>
     </row>
@@ -2684,7 +2680,7 @@
       <c r="C96" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96" s="1">
         <v>96.0</v>
       </c>
     </row>
@@ -2698,7 +2694,7 @@
       <c r="C97" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97" s="1">
         <v>97.0</v>
       </c>
     </row>
@@ -2712,7 +2708,7 @@
       <c r="C98" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E98" s="2">
+      <c r="E98" s="1">
         <v>98.0</v>
       </c>
     </row>
@@ -2723,10 +2719,10 @@
       <c r="B99" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E99" s="2">
+      <c r="E99" s="1">
         <v>99.0</v>
       </c>
     </row>
@@ -2740,7 +2736,7 @@
       <c r="C100" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E100" s="2">
+      <c r="E100" s="1">
         <v>100.0</v>
       </c>
     </row>
@@ -2754,7 +2750,7 @@
       <c r="C101" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E101" s="2">
+      <c r="E101" s="1">
         <v>101.0</v>
       </c>
     </row>
@@ -2768,7 +2764,7 @@
       <c r="C102" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E102" s="2">
+      <c r="E102" s="1">
         <v>102.0</v>
       </c>
     </row>
@@ -2782,7 +2778,7 @@
       <c r="C103" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E103" s="2">
+      <c r="E103" s="1">
         <v>103.0</v>
       </c>
     </row>
@@ -2796,7 +2792,7 @@
       <c r="C104" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104" s="1">
         <v>104.0</v>
       </c>
     </row>
@@ -2810,7 +2806,7 @@
       <c r="C105" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E105" s="1">
         <v>105.0</v>
       </c>
     </row>
@@ -2821,10 +2817,10 @@
       <c r="B106" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E106" s="2">
+      <c r="E106" s="1">
         <v>106.0</v>
       </c>
     </row>
@@ -2838,7 +2834,7 @@
       <c r="C107" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E107" s="1">
         <v>107.0</v>
       </c>
     </row>
@@ -2852,7 +2848,7 @@
       <c r="C108" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E108" s="2">
+      <c r="E108" s="1">
         <v>108.0</v>
       </c>
     </row>
@@ -2866,7 +2862,7 @@
       <c r="C109" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E109" s="2">
+      <c r="E109" s="1">
         <v>109.0</v>
       </c>
     </row>
@@ -2880,7 +2876,7 @@
       <c r="C110" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E110" s="2">
+      <c r="E110" s="1">
         <v>110.0</v>
       </c>
     </row>
@@ -2894,7 +2890,7 @@
       <c r="C111" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E111" s="2">
+      <c r="E111" s="1">
         <v>111.0</v>
       </c>
     </row>
@@ -2908,7 +2904,7 @@
       <c r="C112" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E112" s="2">
+      <c r="E112" s="1">
         <v>112.0</v>
       </c>
     </row>
@@ -2922,7 +2918,7 @@
       <c r="C113" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113" s="1">
         <v>113.0</v>
       </c>
     </row>
@@ -2936,7 +2932,7 @@
       <c r="C114" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E114" s="1">
         <v>114.0</v>
       </c>
     </row>
@@ -2950,7 +2946,7 @@
       <c r="C115" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E115" s="2">
+      <c r="E115" s="1">
         <v>115.0</v>
       </c>
     </row>
@@ -2964,7 +2960,7 @@
       <c r="C116" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E116" s="2">
+      <c r="E116" s="1">
         <v>116.0</v>
       </c>
     </row>
@@ -2972,13 +2968,13 @@
       <c r="A117" s="1">
         <v>5.0</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="1" t="s">
         <v>232</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E117" s="2">
+      <c r="E117" s="1">
         <v>117.0</v>
       </c>
     </row>
@@ -2992,7 +2988,7 @@
       <c r="C118" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E118" s="2">
+      <c r="E118" s="1">
         <v>118.0</v>
       </c>
     </row>
@@ -3006,7 +3002,7 @@
       <c r="C119" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E119" s="2">
+      <c r="E119" s="1">
         <v>119.0</v>
       </c>
     </row>
@@ -3020,7 +3016,7 @@
       <c r="C120" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E120" s="2">
+      <c r="E120" s="1">
         <v>120.0</v>
       </c>
     </row>
@@ -3034,7 +3030,7 @@
       <c r="C121" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E121" s="2">
+      <c r="E121" s="1">
         <v>121.0</v>
       </c>
     </row>
@@ -3048,7 +3044,7 @@
       <c r="C122" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E122" s="2">
+      <c r="E122" s="1">
         <v>122.0</v>
       </c>
     </row>
@@ -3062,7 +3058,7 @@
       <c r="C123" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E123" s="2">
+      <c r="E123" s="1">
         <v>123.0</v>
       </c>
     </row>
@@ -3076,7 +3072,7 @@
       <c r="C124" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E124" s="2">
+      <c r="E124" s="1">
         <v>124.0</v>
       </c>
     </row>
@@ -3090,7 +3086,7 @@
       <c r="C125" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E125" s="2">
+      <c r="E125" s="1">
         <v>125.0</v>
       </c>
     </row>
@@ -3104,26 +3100,26 @@
       <c r="C126" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E126" s="2">
+      <c r="E126" s="1">
         <v>126.0</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B127" s="2" t="s">
+      <c r="A127" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E127" s="2">
+      <c r="E127" s="1">
         <v>127.0</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="2">
+      <c r="A128" s="1">
         <v>6.0</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -3132,12 +3128,12 @@
       <c r="C128" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E128" s="2">
+      <c r="E128" s="1">
         <v>128.0</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="2">
+      <c r="A129" s="1">
         <v>6.0</v>
       </c>
       <c r="B129" s="1" t="s">
@@ -3146,26 +3142,26 @@
       <c r="C129" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E129" s="2">
+      <c r="E129" s="1">
         <v>129.0</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="2">
+      <c r="A130" s="1">
         <v>6.0</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E130" s="2">
+      <c r="E130" s="1">
         <v>130.0</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="2">
+      <c r="A131" s="1">
         <v>6.0</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -3174,12 +3170,12 @@
       <c r="C131" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E131" s="2">
+      <c r="E131" s="1">
         <v>131.0</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="2">
+      <c r="A132" s="1">
         <v>6.0</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -3188,651 +3184,651 @@
       <c r="C132" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E132" s="2">
+      <c r="E132" s="1">
         <v>132.0</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B133" s="2" t="s">
+      <c r="A133" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E133" s="2">
+      <c r="E133" s="1">
         <v>133.0</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B134" s="2" t="s">
+      <c r="A134" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E134" s="2">
+      <c r="E134" s="1">
         <v>134.0</v>
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B135" s="2" t="s">
+      <c r="A135" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E135" s="2">
+      <c r="E135" s="1">
         <v>135.0</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B136" s="2" t="s">
+      <c r="A136" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E136" s="2">
+      <c r="E136" s="1">
         <v>136.0</v>
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B137" s="2" t="s">
+      <c r="A137" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E137" s="2">
+      <c r="E137" s="1">
         <v>137.0</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B138" s="2" t="s">
+      <c r="A138" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E138" s="2">
+      <c r="E138" s="1">
         <v>138.0</v>
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B139" s="2" t="s">
+      <c r="A139" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E139" s="2">
+      <c r="E139" s="1">
         <v>139.0</v>
       </c>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B140" s="2" t="s">
+      <c r="A140" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E140" s="2">
+      <c r="E140" s="1">
         <v>140.0</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B141" s="2" t="s">
+      <c r="A141" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C141" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E141" s="2">
+      <c r="E141" s="1">
         <v>141.0</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B142" s="2" t="s">
+      <c r="A142" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E142" s="2">
+      <c r="E142" s="1">
         <v>142.0</v>
       </c>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B143" s="2" t="s">
+      <c r="A143" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C143" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E143" s="2">
+      <c r="E143" s="1">
         <v>143.0</v>
       </c>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B144" s="2" t="s">
+      <c r="A144" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="C144" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E144" s="2">
+      <c r="E144" s="1">
         <v>144.0</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B145" s="2" t="s">
+      <c r="A145" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C145" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E145" s="2">
+      <c r="E145" s="1">
         <v>145.0</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B146" s="2" t="s">
+      <c r="A146" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C146" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="E146" s="2">
+      <c r="E146" s="1">
         <v>146.0</v>
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B147" s="2" t="s">
+      <c r="A147" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="C147" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E147" s="2">
+      <c r="E147" s="1">
         <v>147.0</v>
       </c>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B148" s="2" t="s">
+      <c r="A148" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="C148" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E148" s="2">
+      <c r="E148" s="1">
         <v>148.0</v>
       </c>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B149" s="2" t="s">
+      <c r="A149" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C149" s="2" t="s">
+      <c r="C149" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E149" s="2">
+      <c r="E149" s="1">
         <v>149.0</v>
       </c>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B150" s="2" t="s">
+      <c r="A150" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="C150" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E150" s="2">
+      <c r="E150" s="1">
         <v>150.0</v>
       </c>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B151" s="2" t="s">
+      <c r="A151" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="C151" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E151" s="2">
+      <c r="E151" s="1">
         <v>151.0</v>
       </c>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B152" s="2" t="s">
+      <c r="A152" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C152" s="2" t="s">
+      <c r="C152" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E152" s="2">
+      <c r="E152" s="1">
         <v>152.0</v>
       </c>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B153" s="2" t="s">
+      <c r="A153" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="C153" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E153" s="2">
+      <c r="E153" s="1">
         <v>153.0</v>
       </c>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B154" s="2" t="s">
+      <c r="A154" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C154" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="E154" s="2">
+      <c r="E154" s="1">
         <v>154.0</v>
       </c>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B155" s="2" t="s">
+      <c r="A155" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="C155" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="E155" s="2">
+      <c r="E155" s="1">
         <v>155.0</v>
       </c>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B156" s="2" t="s">
+      <c r="A156" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C156" s="2" t="s">
+      <c r="C156" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="E156" s="2">
+      <c r="E156" s="1">
         <v>156.0</v>
       </c>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B157" s="2" t="s">
+      <c r="A157" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C157" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="E157" s="2">
+      <c r="E157" s="1">
         <v>157.0</v>
       </c>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B158" s="2" t="s">
+      <c r="A158" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="C158" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="E158" s="2">
+      <c r="E158" s="1">
         <v>158.0</v>
       </c>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B159" s="2" t="s">
+      <c r="A159" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C159" s="2" t="s">
+      <c r="C159" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="E159" s="2">
+      <c r="E159" s="1">
         <v>159.0</v>
       </c>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B160" s="2" t="s">
+      <c r="A160" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="C160" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="E160" s="2">
+      <c r="E160" s="1">
         <v>160.0</v>
       </c>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B161" s="2" t="s">
+      <c r="A161" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C161" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="E161" s="2">
+      <c r="E161" s="1">
         <v>161.0</v>
       </c>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B162" s="2" t="s">
+      <c r="A162" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E162" s="2">
+      <c r="E162" s="1">
         <v>162.0</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B163" s="2" t="s">
+      <c r="A163" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B163" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C163" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E163" s="2">
+      <c r="E163" s="1">
         <v>163.0</v>
       </c>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B164" s="2" t="s">
+      <c r="A164" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C164" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E164" s="2">
+      <c r="E164" s="1">
         <v>164.0</v>
       </c>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B165" s="2" t="s">
+      <c r="A165" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="C165" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E165" s="2">
+      <c r="E165" s="1">
         <v>165.0</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B166" s="2" t="s">
+      <c r="A166" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C166" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E166" s="2">
+      <c r="E166" s="1">
         <v>166.0</v>
       </c>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B167" s="2" t="s">
+      <c r="A167" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C167" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E167" s="2">
+      <c r="E167" s="1">
         <v>167.0</v>
       </c>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B168" s="2" t="s">
+      <c r="A168" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B168" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="C168" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E168" s="2">
+      <c r="E168" s="1">
         <v>168.0</v>
       </c>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B169" s="2" t="s">
+      <c r="A169" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C169" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E169" s="2">
+      <c r="E169" s="1">
         <v>169.0</v>
       </c>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B170" s="2" t="s">
+      <c r="A170" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="C170" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E170" s="2">
+      <c r="E170" s="1">
         <v>170.0</v>
       </c>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B171" s="2" t="s">
+      <c r="A171" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B171" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="E171" s="2">
+      <c r="E171" s="1">
         <v>171.0</v>
       </c>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B172" s="2" t="s">
+      <c r="A172" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B172" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C172" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E172" s="2">
+      <c r="E172" s="1">
         <v>172.0</v>
       </c>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B173" s="2" t="s">
+      <c r="A173" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B173" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C173" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="E173" s="2">
+      <c r="E173" s="1">
         <v>173.0</v>
       </c>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B174" s="2" t="s">
+      <c r="A174" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B174" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C174" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E174" s="2">
+      <c r="E174" s="1">
         <v>174.0</v>
       </c>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B175" s="2" t="s">
+      <c r="A175" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C175" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E175" s="2">
+      <c r="E175" s="1">
         <v>175.0</v>
       </c>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B176" s="2" t="s">
+      <c r="A176" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C176" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="E176" s="2">
+      <c r="E176" s="1">
         <v>176.0</v>
       </c>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B177" s="2" t="s">
+      <c r="A177" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B177" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C177" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="E177" s="2">
+      <c r="E177" s="1">
         <v>177.0</v>
       </c>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B178" s="2" t="s">
+      <c r="A178" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="C178" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E178" s="2">
+      <c r="E178" s="1">
         <v>178.0</v>
       </c>
     </row>

</xml_diff>